<commit_message>
cập nhật chức năng thêm, sửa, import sinh viên
</commit_message>
<xml_diff>
--- a/public/file/import-student.xlsx
+++ b/public/file/import-student.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -86,9 +86,6 @@
     <t>62TH5</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Nguyễn Quang Hưng</t>
   </si>
   <si>
@@ -117,36 +114,6 @@
   </si>
   <si>
     <t>Vũ Tiến Mạnh</t>
-  </si>
-  <si>
-    <t>2051060544@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063502@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063652@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063752@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063562@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063563@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063516@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063812@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063842@e.tlu.edu.vn</t>
-  </si>
-  <si>
-    <t>2051063977@e.tlu.edu.vn</t>
   </si>
   <si>
     <t>12-07-2002</t>
@@ -177,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,14 +156,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,38 +198,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,15 +502,16 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -568,21 +520,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1"/>
@@ -593,290 +542,259 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="7">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6">
         <v>2051060544</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="7">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6">
         <v>2051063502</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="3"/>
+      <c r="F3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="7">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6">
         <v>2051063652</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="3"/>
+      <c r="F4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="7">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6">
         <v>2051063752</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="3"/>
+      <c r="F5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6">
         <v>2051063562</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="3"/>
+      <c r="F6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6">
         <v>2051063563</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="3"/>
+      <c r="F7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="7">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6">
         <v>2051063516</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="3"/>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="3"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6">
         <v>2051063812</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="3"/>
+      <c r="F9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6">
         <v>2051063842</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="3"/>
+      <c r="F10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6">
         <v>2051063977</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="3"/>
+      <c r="F11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="9"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -953,19 +871,7 @@
       <c r="K18" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>